<commit_message>
Updated splits and dates
</commit_message>
<xml_diff>
--- a/brand_splits.xlsx
+++ b/brand_splits.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ammar.aamir\Documents\plan-server-flask\processthesesheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ammar.aamir\Documents\MSyper-cloud\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7512" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7512"/>
   </bookViews>
   <sheets>
     <sheet name="Cluster TG Working" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cluster TG Working'!$B$2:$J$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cluster TG Working'!$B$2:$J$58</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="142">
   <si>
     <t>Category</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Beverages</t>
   </si>
   <si>
-    <t>Brooke Bond Supreme</t>
-  </si>
-  <si>
     <t>Skin Cleansing</t>
   </si>
   <si>
@@ -436,12 +433,33 @@
   </si>
   <si>
     <t>Lux Valentina</t>
+  </si>
+  <si>
+    <t>Brooke Bond Supreme (NC)</t>
+  </si>
+  <si>
+    <t>Brooke Bond Supreme (AKC)</t>
+  </si>
+  <si>
+    <t>Brooke Bond Supreme (Sachet)</t>
+  </si>
+  <si>
+    <t>Walls Cornetto Core</t>
+  </si>
+  <si>
+    <t>Walls Feast</t>
+  </si>
+  <si>
+    <t>Walls Donut</t>
+  </si>
+  <si>
+    <t>Walls Choc Bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1034,11 +1052,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,33 +1085,33 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="G2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:11" s="1" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>3</v>
+        <v>135</v>
       </c>
       <c r="D3" s="8">
         <v>0.1</v>
@@ -1121,66 +1139,66 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="14">
+      <c r="C4" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="8">
         <v>0.1</v>
       </c>
-      <c r="E4" s="14">
-        <v>0.08</v>
-      </c>
-      <c r="F4" s="14">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G4" s="14">
-        <v>0.18</v>
-      </c>
-      <c r="H4" s="14">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I4" s="14">
+      <c r="E4" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="G4" s="8">
         <v>0.2</v>
       </c>
-      <c r="J4" s="17">
+      <c r="H4" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="J4" s="15">
         <v>0.02</v>
       </c>
       <c r="K4" s="20">
-        <f t="shared" ref="K4:K53" si="0">SUM(D4:J4)</f>
+        <f>SUM(D4:J4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="14">
+      <c r="C5" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="F5" s="8">
         <v>0.15</v>
       </c>
-      <c r="E5" s="14">
-        <v>0.05</v>
-      </c>
-      <c r="F5" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="G5" s="14">
+      <c r="G5" s="8">
         <v>0.2</v>
       </c>
-      <c r="H5" s="14">
-        <v>0.3</v>
-      </c>
-      <c r="I5" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="J5" s="17">
-        <v>0</v>
+      <c r="H5" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.16</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0.02</v>
       </c>
       <c r="K5" s="20">
         <f>SUM(D5:J5)</f>
@@ -1191,140 +1209,140 @@
       <c r="B6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="11">
+      <c r="C6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="14">
         <v>0.1</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="14">
         <v>0.08</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="14">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="14">
         <v>0.18</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="14">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="14">
         <v>0.2</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="17">
         <v>0.02</v>
       </c>
       <c r="K6" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K6:K58" si="0">SUM(D6:J6)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="11">
-        <v>0.18</v>
-      </c>
-      <c r="E7" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="F7" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="G7" s="11">
+      <c r="B7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="G7" s="14">
         <v>0.2</v>
       </c>
-      <c r="H7" s="11">
-        <v>0.21</v>
-      </c>
-      <c r="I7" s="11">
-        <v>0.17</v>
-      </c>
-      <c r="J7" s="16">
+      <c r="H7" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="I7" s="14">
+        <v>0.2</v>
+      </c>
+      <c r="J7" s="17">
         <v>0</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="20">
         <f>SUM(D7:J7)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
-        <v>11</v>
+      <c r="B8" s="12" t="s">
+        <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D8" s="11">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="E8" s="11">
-        <v>0.12</v>
+        <v>0.08</v>
       </c>
       <c r="F8" s="11">
         <v>0.14000000000000001</v>
       </c>
       <c r="G8" s="11">
-        <v>0.22</v>
+        <v>0.18</v>
       </c>
       <c r="H8" s="11">
-        <v>0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I8" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="J8" s="16">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="K8" s="20">
-        <f t="shared" ref="K8" si="1">SUM(D8:J8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="D9" s="11">
-        <v>0.13</v>
+        <v>0.18</v>
       </c>
       <c r="E9" s="11">
         <v>0.12</v>
       </c>
       <c r="F9" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="G9" s="11">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="H9" s="11">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="I9" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="J9" s="16">
-        <v>0.03</v>
-      </c>
-      <c r="K9" s="20">
-        <f t="shared" ref="K9:K11" si="2">SUM(D9:J9)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <f>SUM(D9:J9)</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>129</v>
       </c>
       <c r="D10" s="11">
         <v>0.13</v>
@@ -1348,16 +1366,16 @@
         <v>0.03</v>
       </c>
       <c r="K10" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K10" si="1">SUM(D10:J10)</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D11" s="11">
         <v>0.13</v>
@@ -1381,103 +1399,103 @@
         <v>0.03</v>
       </c>
       <c r="K11" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K11:K13" si="2">SUM(D11:J11)</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="E12" s="14">
-        <v>0.08</v>
-      </c>
-      <c r="F12" s="14">
+        <v>128</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="F12" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G12" s="14">
-        <v>0.18</v>
-      </c>
-      <c r="H12" s="14">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I12" s="14">
-        <v>0.2</v>
-      </c>
-      <c r="J12" s="17">
-        <v>0.02</v>
+      <c r="G12" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J12" s="16">
+        <v>0.03</v>
       </c>
       <c r="K12" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="19" t="s">
         <v>10</v>
       </c>
+      <c r="C13" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="D13" s="11">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="E13" s="11">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="F13" s="11">
         <v>0.14000000000000001</v>
       </c>
       <c r="G13" s="11">
-        <v>0.18</v>
+        <v>0.22</v>
       </c>
       <c r="H13" s="11">
-        <v>0.28000000000000003</v>
+        <v>0.22</v>
       </c>
       <c r="I13" s="11">
-        <v>0.16</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J13" s="16">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="K13" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="E14" s="11">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="14">
         <v>0.1</v>
       </c>
-      <c r="F14" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="G14" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="H14" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="I14" s="11">
+      <c r="E14" s="14">
+        <v>0.08</v>
+      </c>
+      <c r="F14" s="14">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0.18</v>
+      </c>
+      <c r="H14" s="14">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I14" s="14">
         <v>0.2</v>
       </c>
-      <c r="J14" s="16">
-        <v>0</v>
+      <c r="J14" s="17">
+        <v>0.02</v>
       </c>
       <c r="K14" s="20">
         <f t="shared" si="0"/>
@@ -1486,31 +1504,31 @@
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>18</v>
-      </c>
       <c r="D15" s="11">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E15" s="11">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F15" s="11">
         <v>0.14000000000000001</v>
       </c>
       <c r="G15" s="11">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="H15" s="11">
-        <v>0.26</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I15" s="11">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="J15" s="16">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="K15" s="20">
         <f t="shared" si="0"/>
@@ -1519,43 +1537,43 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>19</v>
+        <v>132</v>
       </c>
       <c r="D16" s="11">
-        <v>0.11</v>
+        <v>0.05</v>
       </c>
       <c r="E16" s="11">
         <v>0.1</v>
       </c>
       <c r="F16" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="G16" s="11">
-        <v>0.19</v>
+        <v>0.3</v>
       </c>
       <c r="H16" s="11">
-        <v>0.26</v>
+        <v>0.3</v>
       </c>
       <c r="I16" s="11">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="J16" s="16">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="K16" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D17" s="11">
         <v>0.11</v>
@@ -1583,12 +1601,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" s="11">
         <v>0.11</v>
@@ -1616,12 +1634,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D19" s="11">
         <v>0.11</v>
@@ -1649,12 +1667,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D20" s="11">
         <v>0.11</v>
@@ -1682,78 +1700,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="D21" s="11">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E21" s="11">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="F21" s="11">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G21" s="11">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="H21" s="11">
         <v>0.26</v>
       </c>
       <c r="I21" s="11">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="J21" s="16">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="K21" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>80</v>
+        <v>8</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>24</v>
       </c>
       <c r="D22" s="11">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="E22" s="11">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="F22" s="11">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G22" s="11">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="H22" s="11">
         <v>0.26</v>
       </c>
       <c r="I22" s="11">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="J22" s="16">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="K22" s="20">
-        <f t="shared" ref="K22" si="3">SUM(D22:J22)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>75</v>
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="D23" s="11">
         <v>0.12</v>
@@ -1777,16 +1795,16 @@
         <v>0.04</v>
       </c>
       <c r="K23" s="20">
-        <f t="shared" ref="K23:K24" si="4">SUM(D23:J23)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>96</v>
+        <v>8</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="D24" s="11">
         <v>0.12</v>
@@ -1810,16 +1828,16 @@
         <v>0.04</v>
       </c>
       <c r="K24" s="20">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+        <f t="shared" ref="K24" si="3">SUM(D24:J24)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="34" t="s">
-        <v>76</v>
+        <v>8</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>74</v>
       </c>
       <c r="D25" s="11">
         <v>0.12</v>
@@ -1843,67 +1861,67 @@
         <v>0.04</v>
       </c>
       <c r="K25" s="20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K25:K26" si="4">SUM(D25:J25)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>131</v>
+        <v>8</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>95</v>
       </c>
       <c r="D26" s="11">
         <v>0.12</v>
       </c>
       <c r="E26" s="11">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="F26" s="11">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G26" s="11">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="H26" s="11">
-        <v>0.23</v>
+        <v>0.26</v>
       </c>
       <c r="I26" s="11">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="J26" s="16">
         <v>0.04</v>
       </c>
       <c r="K26" s="20">
-        <f t="shared" ref="K26" si="5">SUM(D26:J26)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>132</v>
+        <v>8</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>75</v>
       </c>
       <c r="D27" s="11">
         <v>0.12</v>
       </c>
       <c r="E27" s="11">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="F27" s="11">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="G27" s="11">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="H27" s="11">
-        <v>0.23</v>
+        <v>0.26</v>
       </c>
       <c r="I27" s="11">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="J27" s="16">
         <v>0.04</v>
@@ -1913,78 +1931,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="D28" s="11">
         <v>0.12</v>
       </c>
       <c r="E28" s="11">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="F28" s="11">
         <v>0.1</v>
       </c>
       <c r="G28" s="11">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="H28" s="11">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="I28" s="11">
         <v>0.2</v>
       </c>
       <c r="J28" s="16">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="K28" s="20">
-        <f t="shared" ref="K28" si="6">SUM(D28:J28)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K28" si="5">SUM(D28:J28)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="D29" s="11">
         <v>0.12</v>
       </c>
       <c r="E29" s="11">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="F29" s="11">
         <v>0.1</v>
       </c>
       <c r="G29" s="11">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="H29" s="11">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="I29" s="11">
         <v>0.2</v>
       </c>
       <c r="J29" s="16">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="K29" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="D30" s="11">
         <v>0.12</v>
@@ -1996,65 +2014,64 @@
         <v>0.1</v>
       </c>
       <c r="G30" s="11">
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="H30" s="11">
-        <v>0.26</v>
+        <v>0.25</v>
       </c>
       <c r="I30" s="11">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="J30" s="16">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="K30" s="20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="14">
-        <v>0.12</v>
-      </c>
-      <c r="E31" s="14">
-        <v>0.11</v>
-      </c>
-      <c r="F31" s="14">
+        <f t="shared" ref="K30" si="6">SUM(D30:J30)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="E31" s="11">
         <v>0.1</v>
       </c>
-      <c r="G31" s="14">
+      <c r="F31" s="11">
         <v>0.1</v>
       </c>
-      <c r="H31" s="14">
-        <v>0.3</v>
-      </c>
-      <c r="I31" s="14">
-        <v>0.22</v>
-      </c>
-      <c r="J31" s="17">
-        <v>0.05</v>
+      <c r="G31" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="H31" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="J31" s="16">
+        <v>0.03</v>
       </c>
       <c r="K31" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N31" s="18"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" s="9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D32" s="11">
-        <v>0.17</v>
+        <v>0.12</v>
       </c>
       <c r="E32" s="11">
         <v>0.1</v>
@@ -2063,13 +2080,13 @@
         <v>0.1</v>
       </c>
       <c r="G32" s="11">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="H32" s="11">
         <v>0.26</v>
       </c>
       <c r="I32" s="11">
-        <v>0.16</v>
+        <v>0.19</v>
       </c>
       <c r="J32" s="16">
         <v>0.05</v>
@@ -2078,35 +2095,34 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N32" s="18"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="11">
-        <v>0</v>
-      </c>
-      <c r="E33" s="11">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F33" s="11">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G33" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="H33" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="I33" s="11">
-        <v>0.2</v>
-      </c>
-      <c r="J33" s="16">
-        <v>0.06</v>
+      <c r="B33" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="14">
+        <v>0.12</v>
+      </c>
+      <c r="E33" s="14">
+        <v>0.11</v>
+      </c>
+      <c r="F33" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="G33" s="14">
+        <v>0.1</v>
+      </c>
+      <c r="H33" s="14">
+        <v>0.3</v>
+      </c>
+      <c r="I33" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="J33" s="17">
+        <v>0.05</v>
       </c>
       <c r="K33" s="20">
         <f t="shared" si="0"/>
@@ -2116,28 +2132,28 @@
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="D34" s="11">
-        <v>0.12</v>
+        <v>0.17</v>
       </c>
       <c r="E34" s="11">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="F34" s="11">
         <v>0.1</v>
       </c>
       <c r="G34" s="11">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="H34" s="11">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="I34" s="11">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="J34" s="16">
         <v>0.05</v>
@@ -2150,28 +2166,28 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D35" s="11">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="E35" s="11">
-        <v>0.11</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F35" s="11">
-        <v>0.12</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G35" s="11">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="H35" s="11">
-        <v>0.28000000000000003</v>
+        <v>0.4</v>
       </c>
       <c r="I35" s="11">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="J35" s="16">
         <v>0.06</v>
@@ -2184,31 +2200,31 @@
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D36" s="11">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E36" s="11">
         <v>0.11</v>
       </c>
       <c r="F36" s="11">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="G36" s="11">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="H36" s="11">
-        <v>0.28000000000000003</v>
+        <v>0.27</v>
       </c>
       <c r="I36" s="11">
-        <v>0.16</v>
+        <v>0.17</v>
       </c>
       <c r="J36" s="16">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="K36" s="20">
         <f t="shared" si="0"/>
@@ -2216,354 +2232,354 @@
       </c>
       <c r="N36" s="18"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D37" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.11</v>
       </c>
       <c r="E37" s="11">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="F37" s="11">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="G37" s="11">
         <v>0.16</v>
       </c>
       <c r="H37" s="11">
-        <v>0.26</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I37" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="J37" s="16">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="K37" s="20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+        <f t="shared" ref="K37" si="7">SUM(D37:J37)</f>
+        <v>1</v>
+      </c>
+      <c r="N37" s="18"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>34</v>
+        <v>138</v>
       </c>
       <c r="D38" s="11">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E38" s="11">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="F38" s="11">
         <v>0.12</v>
       </c>
       <c r="G38" s="11">
-        <v>0.15</v>
+        <v>0.16</v>
       </c>
       <c r="H38" s="11">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="I38" s="11">
         <v>0.16</v>
       </c>
       <c r="J38" s="16">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="K38" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="N38" s="18"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>103</v>
+        <v>32</v>
       </c>
       <c r="D39" s="11">
-        <v>0.11</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E39" s="11">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="F39" s="11">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="G39" s="11">
         <v>0.16</v>
       </c>
       <c r="H39" s="11">
-        <v>0.28000000000000003</v>
+        <v>0.26</v>
       </c>
       <c r="I39" s="11">
-        <v>0.16</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J39" s="16">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="K39" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="N39" s="18"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D40" s="11">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="E40" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="F40" s="11">
-        <v>0.22</v>
+        <v>0.12</v>
       </c>
       <c r="G40" s="11">
-        <v>0.23</v>
+        <v>0.15</v>
       </c>
       <c r="H40" s="11">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="I40" s="11">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="J40" s="16">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="K40" s="20">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B41" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="E41" s="11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F41" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="G41" s="11">
+        <v>0.23</v>
+      </c>
+      <c r="H41" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="I41" s="11">
+        <v>0.08</v>
+      </c>
+      <c r="J41" s="16">
+        <v>0</v>
+      </c>
+      <c r="K41" s="20">
+        <f t="shared" ref="K41:K44" si="8">SUM(D41:J41)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B41" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41" s="11">
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B42" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E42" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="F42" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G42" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="H42" s="11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I42" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="J42" s="16">
+        <v>0.06</v>
+      </c>
+      <c r="K42" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B43" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E43" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="F43" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G43" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="H43" s="11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I43" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="J43" s="16">
+        <v>0.06</v>
+      </c>
+      <c r="K43" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B44" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="E44" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="F44" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G44" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="H44" s="11">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I44" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="J44" s="16">
+        <v>0.06</v>
+      </c>
+      <c r="K44" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B45" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="E45" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E41" s="11">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F41" s="11">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G41" s="11">
-        <v>0.19</v>
-      </c>
-      <c r="H41" s="11">
+      <c r="F45" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="G45" s="11">
         <v>0.23</v>
       </c>
-      <c r="I41" s="11">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J41" s="16">
-        <v>0.09</v>
-      </c>
-      <c r="K41" s="20">
-        <f t="shared" ref="K41" si="7">SUM(D41:J41)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B42" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="11">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E42" s="11">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F42" s="11">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G42" s="11">
-        <v>0.19</v>
-      </c>
-      <c r="H42" s="11">
-        <v>0.23</v>
-      </c>
-      <c r="I42" s="11">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="J42" s="16">
-        <v>0.09</v>
-      </c>
-      <c r="K42" s="20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D43" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="E43" s="11">
+      <c r="H45" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="I45" s="11">
         <v>0.08</v>
       </c>
-      <c r="F43" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="G43" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="H43" s="11">
-        <v>0.26</v>
-      </c>
-      <c r="I43" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="J43" s="16">
-        <v>0.12</v>
-      </c>
-      <c r="K43" s="20">
-        <f t="shared" ref="K43" si="8">SUM(D43:J43)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="D44" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="E44" s="11">
-        <v>0.08</v>
-      </c>
-      <c r="F44" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="G44" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="H44" s="11">
-        <v>0.26</v>
-      </c>
-      <c r="I44" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="J44" s="16">
-        <v>0.12</v>
-      </c>
-      <c r="K44" s="20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B45" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="E45" s="11">
-        <v>0.06</v>
-      </c>
-      <c r="F45" s="11">
-        <v>0.17</v>
-      </c>
-      <c r="G45" s="11">
-        <v>0.13</v>
-      </c>
-      <c r="H45" s="11">
-        <v>0.23</v>
-      </c>
-      <c r="I45" s="11">
-        <v>0.2</v>
-      </c>
       <c r="J45" s="16">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="K45" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.99999999999999989</v>
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B46" s="9" t="s">
-        <v>5</v>
+      <c r="B46" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="D46" s="11">
-        <v>0.16</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E46" s="11">
-        <v>0.13</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F46" s="11">
-        <v>0.15</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G46" s="11">
+        <v>0.19</v>
+      </c>
+      <c r="H46" s="11">
+        <v>0.23</v>
+      </c>
+      <c r="I46" s="11">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H46" s="11">
-        <v>0.22</v>
-      </c>
-      <c r="I46" s="11">
-        <v>0.16</v>
-      </c>
       <c r="J46" s="16">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="K46" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K46" si="9">SUM(D46:J46)</f>
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B47" s="9" t="s">
-        <v>5</v>
+      <c r="B47" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D47" s="11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E47" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F47" s="11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G47" s="11">
         <v>0.19</v>
-      </c>
-      <c r="E47" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="F47" s="11">
-        <v>0.12</v>
-      </c>
-      <c r="G47" s="11">
-        <v>0.12</v>
       </c>
       <c r="H47" s="11">
         <v>0.23</v>
@@ -2572,26 +2588,26 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="J47" s="16">
+        <v>0.09</v>
+      </c>
+      <c r="K47" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="E48" s="11">
         <v>0.08</v>
       </c>
-      <c r="K47" s="20">
-        <f>SUM(D47:J47)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B48" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D48" s="11">
-        <v>0.19</v>
-      </c>
-      <c r="E48" s="11">
-        <v>0.12</v>
-      </c>
       <c r="F48" s="11">
         <v>0.12</v>
       </c>
@@ -2599,79 +2615,79 @@
         <v>0.12</v>
       </c>
       <c r="H48" s="11">
-        <v>0.23</v>
+        <v>0.26</v>
       </c>
       <c r="I48" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="J48" s="16">
+        <v>0.12</v>
+      </c>
+      <c r="K48" s="20">
+        <f t="shared" ref="K48" si="10">SUM(D48:J48)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="D49" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="E49" s="11">
         <v>0.08</v>
       </c>
-      <c r="K48" s="20">
-        <f>SUM(D48:J48)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B49" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="11">
-        <v>0.2016</v>
-      </c>
-      <c r="E49" s="11">
-        <v>0.1042</v>
-      </c>
       <c r="F49" s="11">
-        <v>0.17399999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="G49" s="11">
-        <v>0.1245</v>
+        <v>0.12</v>
       </c>
       <c r="H49" s="11">
-        <v>0.20230000000000001</v>
+        <v>0.26</v>
       </c>
       <c r="I49" s="11">
-        <v>0.1278</v>
+        <v>0.15</v>
       </c>
       <c r="J49" s="16">
-        <v>6.4799999999999996E-2</v>
+        <v>0.12</v>
       </c>
       <c r="K49" s="20">
         <f t="shared" si="0"/>
-        <v>0.99920000000000009</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B50" s="9" t="s">
-        <v>5</v>
+      <c r="B50" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D50" s="11">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="E50" s="11">
+        <v>0.06</v>
+      </c>
+      <c r="F50" s="11">
+        <v>0.17</v>
+      </c>
+      <c r="G50" s="11">
         <v>0.13</v>
       </c>
-      <c r="F50" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="G50" s="11">
-        <v>0.14000000000000001</v>
-      </c>
       <c r="H50" s="11">
-        <v>0.22</v>
+        <v>0.23</v>
       </c>
       <c r="I50" s="11">
-        <v>0.16</v>
+        <v>0.2</v>
       </c>
       <c r="J50" s="16">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="K50" s="20">
         <f t="shared" si="0"/>
@@ -2680,31 +2696,31 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>24</v>
+        <v>133</v>
       </c>
       <c r="D51" s="11">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="E51" s="11">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F51" s="11">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="G51" s="11">
-        <v>0.12</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H51" s="11">
-        <v>0.23</v>
+        <v>0.22</v>
       </c>
       <c r="I51" s="11">
-        <v>0.14000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="J51" s="16">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="K51" s="20">
         <f t="shared" si="0"/>
@@ -2713,10 +2729,10 @@
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D52" s="11">
         <v>0.19</v>
@@ -2740,39 +2756,204 @@
         <v>0.08</v>
       </c>
       <c r="K52" s="20">
-        <f t="shared" si="0"/>
+        <f>SUM(D52:J52)</f>
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D53" s="11">
+        <v>0.19</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="F53" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G53" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="H53" s="11">
+        <v>0.23</v>
+      </c>
+      <c r="I53" s="11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J53" s="16">
+        <v>0.08</v>
+      </c>
+      <c r="K53" s="20">
+        <f>SUM(D53:J53)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D53" s="11">
+      <c r="D54" s="11">
+        <v>0.2016</v>
+      </c>
+      <c r="E54" s="11">
+        <v>0.1042</v>
+      </c>
+      <c r="F54" s="11">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="G54" s="11">
+        <v>0.1245</v>
+      </c>
+      <c r="H54" s="11">
+        <v>0.20230000000000001</v>
+      </c>
+      <c r="I54" s="11">
+        <v>0.1278</v>
+      </c>
+      <c r="J54" s="16">
+        <v>6.4799999999999996E-2</v>
+      </c>
+      <c r="K54" s="20">
+        <f t="shared" si="0"/>
+        <v>0.99920000000000009</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B55" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="11">
         <v>0.16</v>
       </c>
-      <c r="E53" s="11">
+      <c r="E55" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="F55" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="G55" s="11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H55" s="11">
+        <v>0.22</v>
+      </c>
+      <c r="I55" s="11">
         <v>0.16</v>
       </c>
-      <c r="F53" s="11">
+      <c r="J55" s="16">
+        <v>0.04</v>
+      </c>
+      <c r="K55" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B56" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D56" s="11">
+        <v>0.19</v>
+      </c>
+      <c r="E56" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="F56" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G56" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="H56" s="11">
+        <v>0.23</v>
+      </c>
+      <c r="I56" s="11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J56" s="16">
+        <v>0.08</v>
+      </c>
+      <c r="K56" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B57" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D57" s="11">
+        <v>0.19</v>
+      </c>
+      <c r="E57" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="F57" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="G57" s="11">
+        <v>0.12</v>
+      </c>
+      <c r="H57" s="11">
+        <v>0.23</v>
+      </c>
+      <c r="I57" s="11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J57" s="16">
+        <v>0.08</v>
+      </c>
+      <c r="K57" s="20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B58" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D58" s="11">
         <v>0.16</v>
       </c>
-      <c r="G53" s="11">
+      <c r="E58" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="F58" s="11">
+        <v>0.16</v>
+      </c>
+      <c r="G58" s="11">
         <v>0.13</v>
       </c>
-      <c r="H53" s="11">
+      <c r="H58" s="11">
         <v>0.22</v>
       </c>
-      <c r="I53" s="11">
+      <c r="I58" s="11">
         <v>0.13</v>
       </c>
-      <c r="J53" s="16">
+      <c r="J58" s="16">
         <v>0.04</v>
       </c>
-      <c r="K53" s="20">
+      <c r="K58" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2784,7 +2965,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2805,33 +2986,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="22" t="s">
+      <c r="D1" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>54</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="21">
         <v>20</v>
@@ -2840,18 +3021,18 @@
         <v>1</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="21">
         <v>20</v>
@@ -2860,18 +3041,18 @@
         <v>1</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>92</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>93</v>
       </c>
       <c r="D4" s="21">
         <v>30</v>
@@ -2880,18 +3061,18 @@
         <v>1</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="21">
         <v>30</v>
@@ -2900,18 +3081,18 @@
         <v>1</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" s="21">
         <v>15</v>
@@ -2920,18 +3101,18 @@
         <v>1</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="21">
         <v>45</v>
@@ -2940,18 +3121,18 @@
         <v>0.5</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="21">
         <v>15</v>
@@ -2960,18 +3141,18 @@
         <v>0.5</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="21">
         <v>45</v>
@@ -2980,18 +3161,18 @@
         <v>0.5</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>61</v>
       </c>
       <c r="D10" s="21">
         <v>21</v>
@@ -3000,18 +3181,18 @@
         <v>0.5</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="21">
         <v>30</v>
@@ -3020,18 +3201,18 @@
         <v>0.2</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="21">
         <v>30</v>
@@ -3040,18 +3221,18 @@
         <v>0.15</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="21">
         <v>30</v>
@@ -3060,18 +3241,18 @@
         <v>0.15</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="21">
         <v>30</v>
@@ -3080,18 +3261,18 @@
         <v>0.5</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" s="21">
         <v>30</v>
@@ -3100,18 +3281,18 @@
         <v>1</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="21">
         <v>30</v>
@@ -3120,18 +3301,18 @@
         <v>1</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="21">
         <v>15</v>
@@ -3140,18 +3321,18 @@
         <v>1</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" s="21">
         <v>30</v>
@@ -3160,18 +3341,18 @@
         <v>1</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D19" s="21">
         <v>40</v>
@@ -3180,18 +3361,18 @@
         <v>1</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" s="21">
         <v>30</v>
@@ -3200,18 +3381,18 @@
         <v>1</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" s="21">
         <v>30</v>
@@ -3220,18 +3401,18 @@
         <v>1</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22" s="21">
         <v>40</v>
@@ -3240,18 +3421,18 @@
         <v>1</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>96</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>97</v>
       </c>
       <c r="D23" s="21">
         <v>30</v>
@@ -3260,18 +3441,18 @@
         <v>1</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D24" s="21">
         <v>21</v>
@@ -3280,19 +3461,19 @@
         <v>0.5</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H24" s="26"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D25" s="21">
         <v>21</v>
@@ -3301,18 +3482,18 @@
         <v>0.5</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="21">
         <v>20</v>
@@ -3321,18 +3502,18 @@
         <v>1</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D27" s="21">
         <v>20</v>
@@ -3341,18 +3522,18 @@
         <v>1</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>99</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="21" t="s">
-        <v>100</v>
       </c>
       <c r="D28" s="21">
         <v>30</v>
@@ -3361,18 +3542,18 @@
         <v>1</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" s="30">
         <v>30</v>
@@ -3381,18 +3562,18 @@
         <v>1</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D30" s="25">
         <v>40</v>
@@ -3401,18 +3582,18 @@
         <v>0.75</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D31" s="25">
         <v>10</v>
@@ -3421,18 +3602,18 @@
         <v>0.25</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32">
         <v>15</v>
@@ -3441,18 +3622,18 @@
         <v>0.25</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D33">
         <v>30</v>
@@ -3461,18 +3642,18 @@
         <v>0.5</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D34">
         <v>20</v>
@@ -3481,18 +3662,18 @@
         <v>0.25</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D35">
         <v>20</v>
@@ -3501,18 +3682,18 @@
         <v>0.5</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D36">
         <v>20</v>
@@ -3521,18 +3702,18 @@
         <v>0.5</v>
       </c>
       <c r="F36" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37">
         <v>30</v>
@@ -3541,18 +3722,18 @@
         <v>0.7</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D38">
         <v>12</v>
@@ -3561,18 +3742,18 @@
         <v>0.3</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D39">
         <v>15</v>
@@ -3581,18 +3762,18 @@
         <v>1</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" t="s">
         <v>115</v>
-      </c>
-      <c r="B40" s="29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C40" t="s">
-        <v>116</v>
       </c>
       <c r="D40">
         <v>7</v>
@@ -3601,18 +3782,18 @@
         <v>1</v>
       </c>
       <c r="F40" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D41">
         <v>10</v>
@@ -3621,18 +3802,18 @@
         <v>1</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D42">
         <v>30</v>
@@ -3641,18 +3822,18 @@
         <v>0.7</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D43">
         <v>15</v>
@@ -3661,18 +3842,18 @@
         <v>0.3</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D44">
         <v>20</v>
@@ -3681,18 +3862,18 @@
         <v>1</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="31" t="s">
         <v>121</v>
-      </c>
-      <c r="B45" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="31" t="s">
-        <v>122</v>
       </c>
       <c r="D45">
         <v>30</v>
@@ -3701,18 +3882,18 @@
         <v>1</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D46">
         <v>15</v>
@@ -3721,18 +3902,18 @@
         <v>1</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" t="s">
         <v>124</v>
-      </c>
-      <c r="B47" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C47" t="s">
-        <v>125</v>
       </c>
       <c r="D47">
         <v>20</v>
@@ -3741,7 +3922,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>